<commit_message>
Java Season 3 Notes and Programs till Sep 22nd
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FLM2ndJuneWS\JavaSeasons3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E0ECEC-4AC0-49F5-B281-8467AF0803F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F565AE-8A2D-43BA-A429-5453C695BC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CBAC835F-06DF-4752-839D-6AFBFFE04C25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CBAC835F-06DF-4752-839D-6AFBFFE04C25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>abc</t>
   </si>
@@ -44,32 +44,53 @@
     <t>java</t>
   </si>
   <si>
-    <t>xyz</t>
-  </si>
-  <si>
     <t>selenium</t>
   </si>
   <si>
     <t>python</t>
   </si>
   <si>
-    <t>Sno</t>
-  </si>
-  <si>
-    <t>emp id</t>
-  </si>
-  <si>
-    <t>ename</t>
-  </si>
-  <si>
-    <t>john</t>
+    <t>reyaz</t>
+  </si>
+  <si>
+    <t>FLM</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://adactinhotelapp.com/</t>
+  </si>
+  <si>
+    <t>implicitWait</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>reyaz0806</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>reyaz123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +100,13 @@
     </font>
     <font>
       <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -105,9 +133,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,9 +451,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596490F0-3488-4A4A-8129-305B0278CB31}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.8" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -434,7 +463,7 @@
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,26 +471,34 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>456</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -471,34 +508,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD5D9A9-8C49-489B-8F84-7136F60EE2F4}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>